<commit_message>
UNS import and export support JSON！
</commit_message>
<xml_diff>
--- a/UnityNamespace/src/main/resources/templates/all-namespace.xlsx
+++ b/UnityNamespace/src/main/resources/templates/all-namespace.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12375" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="6" r:id="rId1"/>
-    <sheet name="Folder" sheetId="7" r:id="rId2"/>
-    <sheet name="relation" sheetId="1" r:id="rId3"/>
-    <sheet name="TimeSeries" sheetId="4" r:id="rId4"/>
+    <sheet name="Label" sheetId="8" r:id="rId2"/>
+    <sheet name="Folder" sheetId="7" r:id="rId3"/>
+    <sheet name="File-timeseries" sheetId="4" r:id="rId4"/>
+    <sheet name="File-relation" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,48 +31,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>alias</t>
+  </si>
+  <si>
     <t>fields</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
-    <t>demo</t>
+    <t>template1</t>
   </si>
   <si>
     <t>[{"name":"t0","type":"int"},
 {"name":"t1","type":"long"}]</t>
   </si>
   <si>
-    <t>demo/g1</t>
+    <t>template2</t>
   </si>
   <si>
     <t>↓↓↓ Please enter your template information start with row 5 ↓↓↓</t>
   </si>
   <si>
-    <t>alias</t>
-  </si>
-  <si>
-    <t>template</t>
-  </si>
-  <si>
-    <t>demo/</t>
-  </si>
-  <si>
-    <t>demo/g1/</t>
+    <t>label1</t>
+  </si>
+  <si>
+    <t>label2</t>
+  </si>
+  <si>
+    <t>↓↓↓ Please enter your label start with row 5 ↓↓↓</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>templateAlias</t>
+  </si>
+  <si>
+    <t>folder1/</t>
+  </si>
+  <si>
+    <t>folder1/folder2/</t>
   </si>
   <si>
     <t>↓↓↓ Please enter your folder information start with row 5 ↓↓↓</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
     <t>mockData</t>
   </si>
   <si>
@@ -84,16 +94,40 @@
     <t>label</t>
   </si>
   <si>
+    <t>folder1/tag1</t>
+  </si>
+  <si>
+    <t>tag1_xxx</t>
+  </si>
+  <si>
+    <t>[{"name":"t0","type":"int"},{"name":"t1","type":"long"},{"name":"t2","type":"float"}]</t>
+  </si>
+  <si>
+    <t>folder1/tag2</t>
+  </si>
+  <si>
+    <t>tag2_xxx</t>
+  </si>
+  <si>
+    <t>[{"name":"t0","type":"int","index":0},{"name":"t1","type":"long","index":1},{"name":"t2","type":"float"}]</t>
+  </si>
+  <si>
     <t>label1,label2</t>
   </si>
   <si>
     <t>↓↓↓ Please enter your namespace information start with row 5 ↓↓↓</t>
   </si>
   <si>
-    <t>[{"name":"t0","type":"int"},{"name":"t1","type":"long"},{"name":"t2","type":"float"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"t0","type":"int","index":0},{"name":"t1","type":"long","index":1},{"name":"t2","type":"float"}]</t>
+    <t>folder1/rel1</t>
+  </si>
+  <si>
+    <t>rel1_xxx</t>
+  </si>
+  <si>
+    <t>folder1/rel2</t>
+  </si>
+  <si>
+    <t>rel2_xxx</t>
   </si>
 </sst>
 </file>
@@ -497,7 +531,9 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -510,9 +546,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -805,28 +839,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -835,6 +866,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1147,56 +1181,63 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="21.75" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" ht="54" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="54" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" ht="54" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" ht="54" spans="1:4">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1206,13 +1247,50 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="121.5" spans="1:1">
+      <c r="A4" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="3" width="33.125" customWidth="1"/>
     <col min="4" max="4" width="58.375" customWidth="1"/>
@@ -1220,64 +1298,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" ht="27" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="27" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="6"/>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="4:4">
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="4:4">
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="4:4">
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="4:4">
-      <c r="D8" s="9"/>
+      <c r="A4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1288,132 +1354,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
-  <cols>
-    <col min="1" max="3" width="33.125" customWidth="1"/>
-    <col min="4" max="4" width="58.375" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="9" max="9" width="13.5916666666667" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" ht="27" spans="1:9">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" ht="18" customHeight="1" spans="1:9">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" ht="23" customHeight="1" spans="1:9">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="4:4">
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="4:4">
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="4:4">
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="4:4">
-      <c r="D8" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A4:I4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
@@ -1426,41 +1373,43 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" ht="40.5" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1470,14 +1419,16 @@
     </row>
     <row r="3" ht="64" customHeight="1" spans="1:9">
       <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="6"/>
+      <c r="D3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="8"/>
       <c r="F3" s="5" t="b">
         <v>0</v>
       </c>
@@ -1488,21 +1439,21 @@
         <v>0</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="A4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1511,4 +1462,115 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="$A5:$XFD30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="3" width="33.125" customWidth="1"/>
+    <col min="4" max="4" width="58.375" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="9" max="9" width="13.5916666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" ht="27" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" ht="18" customHeight="1" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" ht="23" customHeight="1" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>